<commit_message>
增加 201 - 读写 CMOS RAM
</commit_message>
<xml_diff>
--- a/指令、寄存器、标志寄存器总结.xlsx
+++ b/指令、寄存器、标志寄存器总结.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mi\Desktop\Programma\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94883500-6F1B-4863-B5A7-B7CBA3956F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43873D17-0951-485F-93E8-B205C116046E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="1170" windowWidth="36405" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="指令" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
   <si>
     <t>位</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -797,12 +797,72 @@
     <t>retf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>out 端口, al/ax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将 al/ax中的数据送入端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in al/ax, 端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将 端口 中的信息送入 al/ax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑(左移)位移指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑(右移)位移指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mov al, 01001000B
+shl al, 1                    --&gt; 将 al 中的数据左移一位，移出的一位放在CF中。
+                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>如果位移的位数大于1时，必须将移动位数放在 CL 中</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,6 +945,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1105,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1217,6 +1292,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1498,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1873,6 +1954,47 @@
     <row r="57" spans="1:3" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" s="11" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +2108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC954F4D-A1FD-470B-8B78-559B169FBECA}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>